<commit_message>
Add all tree except rotate
</commit_message>
<xml_diff>
--- a/08_assoc_array/metrics.xlsx
+++ b/08_assoc_array/metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zholu\Documents\Programming\ooap1\08_assoc_array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9F72EC-0178-4846-BB35-3F915657563C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC3C755-F37A-459A-A25C-5C636091C4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>Тип</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>невнимательность к типам</t>
+  </si>
+  <si>
+    <t>переделал АТД</t>
+  </si>
+  <si>
+    <t>неверное проектирование АТД</t>
+  </si>
+  <si>
+    <t>размывание уровней абстракции (недостаток опыта)</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -422,9 +431,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -790,7 +796,7 @@
       </c>
       <c r="B3" s="3">
         <f ca="1">SUM(C16:C18)</f>
-        <v>243.00000000000023</v>
+        <v>292.00000000000023</v>
       </c>
       <c r="C3" s="3">
         <f>SUM(B16:B18)</f>
@@ -801,7 +807,7 @@
       </c>
       <c r="E3" s="20">
         <f t="shared" ref="E3:E7" ca="1" si="0">C3/B3</f>
-        <v>0.98765432098765338</v>
+        <v>0.82191780821917748</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,7 +816,7 @@
       </c>
       <c r="B4" s="3">
         <f ca="1">SUM(C15:C19)</f>
-        <v>256.00000000000023</v>
+        <v>305.00000000000023</v>
       </c>
       <c r="C4" s="3">
         <f>SUM(B15:B19)</f>
@@ -818,7 +824,7 @@
       </c>
       <c r="E4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0937499999999991</v>
+        <v>0.91803278688524526</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,7 +854,7 @@
       </c>
       <c r="B6">
         <f>SUM(E15:E19)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <f>SUM(D15:D19)</f>
@@ -857,7 +863,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="20">
         <f t="shared" si="0"/>
-        <v>1.5714285714285714</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,7 +872,7 @@
       </c>
       <c r="B7" s="10">
         <f ca="1">IF(B4&gt;0,B6/B4*60,0)</f>
-        <v>1.6406249999999984</v>
+        <v>1.5737704918032773</v>
       </c>
       <c r="C7" s="10">
         <f>IF(C4&gt;0,C6/C4*60,0)</f>
@@ -875,7 +881,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4367346938775525</v>
+        <v>1.4977678571428585</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,7 +901,7 @@
       </c>
       <c r="B9" s="10">
         <f>SUM(F15:F19)</f>
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -906,7 +912,7 @@
       </c>
       <c r="B10" s="10">
         <f>IF(B6&gt;0,B9/B6,0)</f>
-        <v>1.1428571428571428</v>
+        <v>7.25</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -975,22 +981,22 @@
       </c>
       <c r="C16" s="3">
         <f ca="1">SUMIF(Сессии!$A$2:$A$10001,$A16,Сессии!$H$2:$H$10001)</f>
-        <v>135.00000000000023</v>
+        <v>144.0000000000002</v>
       </c>
       <c r="D16" s="13">
         <v>3</v>
       </c>
       <c r="E16">
         <f>COUNTIF(Ошибки!$E$2:$E$10001,$A16)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16">
         <f>SUMIF(Ошибки!$E$2:$E$10001,$A16,Ошибки!$F$2:$F$10001)</f>
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="G16">
         <f t="shared" ref="G16:G19" si="1">IF(E16&gt;0,F16/E16,0)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1002,7 +1008,7 @@
       </c>
       <c r="C17" s="3">
         <f ca="1">SUMIF(Сессии!$A$2:$A$10001,$A17,Сессии!$H$2:$H$10001)</f>
-        <v>108.00000000000001</v>
+        <v>148.00000000000003</v>
       </c>
       <c r="D17" s="13">
         <v>5</v>
@@ -1166,11 +1172,11 @@
       </c>
       <c r="C28">
         <f>COUNTIF(Ошибки!$C$2:$C$10001,$A28)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <f>SUMIF(Ошибки!$C$2:$C$10001,$A28,Ошибки!$F$2:$F$10001)</f>
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,7 +1270,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1279,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="25" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
@@ -1293,7 +1299,7 @@
       <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1322,7 +1328,7 @@
       <c r="D2" s="17">
         <v>0.53888888888888886</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>70</v>
       </c>
       <c r="F2" s="12">
@@ -1369,7 +1375,7 @@
       <c r="D4" s="17">
         <v>0.63888888888888895</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>73</v>
       </c>
       <c r="F4" s="12">
@@ -1494,7 +1500,7 @@
       <c r="D13" s="19">
         <v>0.85138888888888886</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="12">
@@ -1527,7 +1533,7 @@
       <c r="D14" s="19">
         <v>0.89583333333333337</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="26" t="s">
         <v>80</v>
       </c>
       <c r="F14" s="12">
@@ -1560,7 +1566,7 @@
       <c r="D15" s="17">
         <v>0.76041666666666663</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="12">
         <f ca="1">IF(I15&gt;0,SUM(OFFSET(F16,0,0,I15,1)),0)</f>
         <v>23</v>
@@ -1574,7 +1580,7 @@
         <v>56.999999999999872</v>
       </c>
       <c r="I15" s="12">
-        <f>MATCH(TRUE,INDEX(((A16:A115="")*(F16:F115="")+(A16:A115&lt;&gt;"")&gt;0),),0)-1</f>
+        <f ca="1">MATCH(TRUE,INDEX(((A16:A115="")*(F16:F115="")+(A16:A115&lt;&gt;"")&gt;0),),0)-1</f>
         <v>7</v>
       </c>
     </row>
@@ -1593,7 +1599,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="E17" s="23" t="s">
         <v>81</v>
@@ -1602,7 +1608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="19"/>
       <c r="D18" s="17"/>
@@ -1616,7 +1622,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19" s="23" t="s">
         <v>81</v>
       </c>
@@ -1624,7 +1630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" s="23" t="s">
         <v>81</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E21" s="23" t="s">
         <v>69</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="19"/>
       <c r="D22" s="17"/>
@@ -1654,22 +1660,72 @@
       <c r="H22" s="18"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="25"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="25"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="15">
+        <v>44929</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0.61944444444444446</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0.62569444444444444</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="12">
+        <f ca="1">IF(I23&gt;0,SUM(OFFSET(F24,0,0,I23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="18">
+        <f t="shared" ref="G23" si="1">IF(D23&lt;&gt;"",(D23-C23)*1440,0)</f>
+        <v>8.999999999999968</v>
+      </c>
+      <c r="H23" s="18">
+        <f ca="1">IF(G23&gt;0,G23-F23,0)</f>
+        <v>8.999999999999968</v>
+      </c>
+      <c r="I23" s="12">
+        <f ca="1">MATCH(TRUE,INDEX(((A24:A123="")*(F24:F123="")+(A24:A123&lt;&gt;"")&gt;0),),0)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="15">
+        <v>44929</v>
+      </c>
+      <c r="C24" s="19">
+        <v>0.62638888888888888</v>
+      </c>
+      <c r="D24" s="19">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="12">
+        <f ca="1">IF(I24&gt;0,SUM(OFFSET(F25,0,0,I24,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" ref="G24" si="2">IF(D24&lt;&gt;"",(D24-C24)*1440,0)</f>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="H24" s="18">
+        <f ca="1">IF(G24&gt;0,G24-F24,0)</f>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="I24" s="12">
+        <f>MATCH(TRUE,INDEX(((A25:A124="")*(F25:F124="")+(A25:A124&lt;&gt;"")&gt;0),),0)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="24"/>
       <c r="F25" s="22"/>
     </row>
   </sheetData>
@@ -1683,13 +1739,13 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="33" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="32" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
@@ -1698,10 +1754,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1721,10 +1777,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="9">
@@ -1744,10 +1800,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="9">
@@ -1767,10 +1823,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="9">
@@ -1790,10 +1846,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="9">
@@ -1813,10 +1869,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="9">
@@ -1836,10 +1892,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="9">
@@ -1859,10 +1915,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>85</v>
       </c>
       <c r="C8" s="9">
@@ -1871,7 +1927,7 @@
       <c r="D8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F8">
@@ -1882,8 +1938,27 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="9">
+        <v>50</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>

</xml_diff>

<commit_message>
Add reflexion for AA
</commit_message>
<xml_diff>
--- a/08_assoc_array/metrics.xlsx
+++ b/08_assoc_array/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zholu\Documents\Programming\ooap1\08_assoc_array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7AFEE6-831B-4D11-B1D6-83CC3D6280ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D376DC2F-5445-44EE-8CDF-97D2CFCA68FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Сводка" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
   <si>
     <t>Тип</t>
   </si>
@@ -802,7 +802,7 @@
       </c>
       <c r="B3" s="3">
         <f ca="1">SUM(C16:C18)</f>
-        <v>531</v>
+        <v>570.99999999999989</v>
       </c>
       <c r="C3" s="3">
         <f>SUM(B16:B18)</f>
@@ -813,7 +813,7 @@
       </c>
       <c r="E3" s="20">
         <f t="shared" ref="E3:E7" ca="1" si="0">C3/B3</f>
-        <v>0.4519774011299435</v>
+        <v>0.42031523642732055</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
       </c>
       <c r="B4" s="3">
         <f ca="1">SUM(C15:C19)</f>
-        <v>544</v>
+        <v>583.99999999999989</v>
       </c>
       <c r="C4" s="3">
         <f>SUM(B15:B19)</f>
@@ -830,7 +830,7 @@
       </c>
       <c r="E4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51470588235294112</v>
+        <v>0.47945205479452063</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
       </c>
       <c r="B7" s="10">
         <f ca="1">IF(B4&gt;0,B6/B4*60,0)</f>
-        <v>1.1029411764705883</v>
+        <v>1.0273972602739727</v>
       </c>
       <c r="C7" s="10">
         <f>IF(C4&gt;0,C6/C4*60,0)</f>
@@ -887,7 +887,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>2.137142857142857</v>
+        <v>2.294285714285714</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="C17" s="3">
         <f ca="1">SUMIF(Сессии!$A$2:$A$10001,$A17,Сессии!$H$2:$H$10001)</f>
-        <v>386.99999999999977</v>
+        <v>426.99999999999966</v>
       </c>
       <c r="D17" s="13">
         <v>5</v>
@@ -1273,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,22 +1864,51 @@
       <c r="C34" s="19">
         <v>0.81944444444444453</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="E34" s="24"/>
       <c r="F34" s="12">
         <f ca="1">IF(I34&gt;0,SUM(OFFSET(F35,0,0,I34,1)),0)</f>
         <v>0</v>
       </c>
       <c r="G34" s="18">
-        <f t="shared" ref="G34" si="5">IF(D34&lt;&gt;"",(D34-C34)*1440,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G34:G35" si="5">IF(D34&lt;&gt;"",(D34-C34)*1440,0)</f>
+        <v>39.999999999999858</v>
       </c>
       <c r="H34" s="18">
-        <f>IF(G34&gt;0,G34-F34,0)</f>
-        <v>0</v>
+        <f ca="1">IF(G34&gt;0,G34-F34,0)</f>
+        <v>39.999999999999858</v>
       </c>
       <c r="I34" s="12">
-        <f>MATCH(TRUE,INDEX(((A35:A134="")*(F35:F134="")+(A35:A134&lt;&gt;"")&gt;0),),0)-1</f>
+        <f ca="1">MATCH(TRUE,INDEX(((A35:A134="")*(F35:F134="")+(A35:A134&lt;&gt;"")&gt;0),),0)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="15">
+        <v>44931</v>
+      </c>
+      <c r="C35" s="19">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="F35" s="12">
+        <f ca="1">IF(I35&gt;0,SUM(OFFSET(F36,0,0,I35,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="18">
+        <f>IF(G35&gt;0,G35-F35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="12">
+        <f>MATCH(TRUE,INDEX(((A36:A135="")*(F36:F135="")+(A36:A135&lt;&gt;"")&gt;0),),0)-1</f>
         <v>0</v>
       </c>
     </row>
@@ -1893,7 +1922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA175472-95AE-4F30-9632-D2B04CFDFBCF}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>